<commit_message>
Added proposed button mappings and some questions/comments
All text added are tagged with [Jason F: ...]
</commit_message>
<xml_diff>
--- a/2022CompetitionBot/Controller Mapping 2022.xlsx
+++ b/2022CompetitionBot/Controller Mapping 2022.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\FRC\2022repo\2022CompetitionBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Personal\4917\2022repo\2022CompetitionBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C49F365-9208-478D-B9B5-8A95BA7BB8ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19290" yWindow="12555" windowWidth="29115" windowHeight="17625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19290" yWindow="12555" windowWidth="29115" windowHeight="17625" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,20 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Up-Shift</t>
   </si>
   <si>
-    <t>Left-Shift</t>
-  </si>
-  <si>
     <t>Down-Shift</t>
   </si>
   <si>
-    <t>Right-Shift</t>
-  </si>
-  <si>
     <t>Kill Everything</t>
   </si>
   <si>
@@ -83,29 +76,247 @@
     <t>Driver Controller</t>
   </si>
   <si>
-    <t>v0.1 (Feb 9, 2022)</t>
-  </si>
-  <si>
-    <t>Spin Up Flywheel?</t>
-  </si>
-  <si>
-    <t>Auto Shoot?</t>
-  </si>
-  <si>
     <t>Expel?</t>
   </si>
   <si>
-    <t>Intake?</t>
-  </si>
-  <si>
     <t>Disable Auto-Shift?</t>
+  </si>
+  <si>
+    <t>v0.1 (Feb 28, 2022)</t>
+  </si>
+  <si>
+    <t>[Jason F: Pivoting Arm Extend?]</t>
+  </si>
+  <si>
+    <t>[Jason F: Pivoting Arm Retract?]</t>
+  </si>
+  <si>
+    <t>[Jason F: Auto shoot?]</t>
+  </si>
+  <si>
+    <t>[Jason F: Spin Up Flyweheel / Shut Down Flywheel?]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Jason F: Pivot Pivoting Arm Left?]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Left-Shift</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Jason F: Stationary Arm Extend?]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Auto Shoot?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Jason F: Stationary Arm Retract?]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF808080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Spin Up Flywheel?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Jason F: Pivot Pivoting Arm Right?]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Right-Shift</t>
+    </r>
+  </si>
+  <si>
+    <t>[Jason F: Auto Climb?]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[Jason F: Intake Toggle?]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Intake?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[Jason F:
+1. As coded, I see that </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Intake</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> puts down intake arm and sucks in cargo only while button is held. On button release, intake arm raises and stops sucking in. Can we make one button press engage intake and alternate button press disengage it, so it is a toggle? </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Expel</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> would, reverse intake rollers while held and return to nromal intake on release if intake was one or back to idel if intake was not on.
+2. Can </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Spin Up Flywheel</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> be a toggle? Use it to pre-spin up the flywheel when anticipating the need to shoot soon. Need a way to shut it down anyway.
+3. Using the typical shift button (left/right) for pivot arm pivoting makes it less likely to accidentally pivot while not climbing (as opposed to using joysticks). Would give better pivot control too (tapping left/right ever so lightly). I'd even abandon shift up/down and use a single </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>General Shift</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> button at competition time if needed.
+]</t>
+    </r>
+  </si>
+  <si>
+    <t>[Jason F: General Shift
+(for competition if needed)?]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -201,13 +412,80 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFCC9900"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -333,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -354,9 +632,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -432,6 +707,37 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,16 +828,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>95760</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1216800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1216801</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>242117</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -566,14 +872,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>86040</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1207080</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1207081</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>320955</xdr:rowOff>
     </xdr:to>
@@ -907,368 +1213,374 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K35"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
-    <col min="4" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1"/>
-    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="19.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="8" max="1024" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="3" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5"/>
+    <row r="3" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="G3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="H4" s="7"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
+      <c r="G4" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="10"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="G5" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="H6" s="11"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="G6" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="H7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="9"/>
+      <c r="G7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="H8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="G8" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="9"/>
+      <c r="G9" s="39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="2:11" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="9"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="34" t="s">
+      <c r="C15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="17" t="s">
+      <c r="D15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="E15" s="17"/>
+      <c r="F15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="C16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="22" t="s">
-        <v>9</v>
-      </c>
       <c r="D16" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E16" s="24"/>
       <c r="F16" s="25"/>
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="27"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>9</v>
+      </c>
       <c r="C17" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="30" t="s">
-        <v>13</v>
+      <c r="C19" s="22" t="s">
+        <v>8</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="31"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="21" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C21" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="23" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="30"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="23" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="H23" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
+      <c r="G23" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="9"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="H27" s="32"/>
-    </row>
-    <row r="28" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="C28" s="9"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="5"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
-      <c r="C30" s="9"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="H30" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="5"/>
+      <c r="G30" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="9"/>
+      <c r="G31" s="15"/>
+    </row>
+    <row r="32" spans="1:9" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="H32" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="H35" s="10"/>
+      <c r="G32" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="G34" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C21:G21"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="A33:G33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -1284,7 +1596,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>

<commit_message>
Update Controller Mapping 2022.xlsx
Added Align and Shoot to Driver Controller
</commit_message>
<xml_diff>
--- a/2022CompetitionBot/Controller Mapping 2022.xlsx
+++ b/2022CompetitionBot/Controller Mapping 2022.xlsx
@@ -22,12 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t xml:space="preserve">Operator Controller</t>
   </si>
   <si>
-    <t xml:space="preserve">v0.3 (Mar 3, 2022)</t>
+    <t xml:space="preserve">v1.0 (Mar 22, 2022)</t>
   </si>
   <si>
     <t xml:space="preserve">Shoot Low</t>
@@ -78,7 +78,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Expel</t>
+    <t xml:space="preserve">Expel?</t>
   </si>
   <si>
     <t xml:space="preserve">Down-Shift</t>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">Auto Shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Align and Shoot</t>
   </si>
   <si>
     <t xml:space="preserve">Turn Left/Right</t>
@@ -669,9 +672,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1216080</xdr:colOff>
+      <xdr:colOff>1215720</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
+      <xdr:rowOff>241560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -686,7 +689,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2615400" y="438480"/>
-          <a:ext cx="5977440" cy="3255120"/>
+          <a:ext cx="5977080" cy="3254760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -707,9 +710,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1206360</xdr:colOff>
+      <xdr:colOff>1206000</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>320760</xdr:rowOff>
+      <xdr:rowOff>320400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -724,7 +727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2605680" y="5740920"/>
-          <a:ext cx="5977440" cy="3303360"/>
+          <a:ext cx="5977080" cy="3303000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -747,7 +750,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1050,7 +1053,9 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
@@ -1059,12 +1064,12 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="G30" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>

</xml_diff>

<commit_message>
Climb Auto Change: Added missing delay and logic to keep robot up to grab traversal rung
</commit_message>
<xml_diff>
--- a/2022CompetitionBot/Controller Mapping 2022.xlsx
+++ b/2022CompetitionBot/Controller Mapping 2022.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t xml:space="preserve">Operator Controller</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t xml:space="preserve">Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Override Wench limits</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
@@ -675,9 +672,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1215360</xdr:colOff>
+      <xdr:colOff>1215720</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>241200</xdr:rowOff>
+      <xdr:rowOff>241560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -692,7 +689,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2615400" y="438480"/>
-          <a:ext cx="5976720" cy="3254400"/>
+          <a:ext cx="5977080" cy="3254760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -713,9 +710,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1205640</xdr:colOff>
+      <xdr:colOff>1206000</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>320040</xdr:rowOff>
+      <xdr:rowOff>320400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -730,7 +727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2605680" y="5740920"/>
-          <a:ext cx="5976720" cy="3302640"/>
+          <a:ext cx="5977080" cy="3303000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -753,7 +750,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -932,7 +929,7 @@
         <v>24</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
@@ -942,13 +939,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="30"/>
@@ -958,13 +955,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="29"/>
       <c r="F18" s="30"/>
@@ -973,13 +970,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="27"/>
       <c r="F19" s="36"/>
@@ -988,7 +985,7 @@
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1006,14 +1003,14 @@
     </row>
     <row r="24" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="G24" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1031,7 +1028,7 @@
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="G26" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1057,7 +1054,7 @@
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="G29" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1067,12 +1064,12 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="G30" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>

</xml_diff>